<commit_message>
Updated Diagram of iterations and UserStoryList
</commit_message>
<xml_diff>
--- a/FVisual_Documentation/UserStoryListe_BacklogItemsErfassung.xlsx
+++ b/FVisual_Documentation/UserStoryListe_BacklogItemsErfassung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sandr\OneDrive - HTL Villach\Schule\Schule\5AHIF\POS1_LIN\Project\FVisual\FVisual_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="489" documentId="13_ncr:1_{1D5C89E9-F122-4CD9-B0A4-16354C845C53}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{465C03F4-BE78-49F3-819C-DA00923E6D9C}"/>
+  <xr:revisionPtr revIDLastSave="647" documentId="13_ncr:1_{1D5C89E9-F122-4CD9-B0A4-16354C845C53}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{35BBFAE0-EEA5-4E26-8EC5-EF0609B039E0}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{DA8F7C48-B531-4135-8DC3-731F75A6B69C}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="150">
   <si>
     <t>Iteration 2</t>
   </si>
@@ -332,18 +332,6 @@
     <t>US - Android Applikation Karte anzeigen</t>
   </si>
   <si>
-    <t>US - Android Applikation Einsätze als Testdaten anzeigen (Ohne DB Zugriff)</t>
-  </si>
-  <si>
-    <t>US - Android Applikation Stützpunkte als Testdaten anzeigen (Ohne DB Zugriff)</t>
-  </si>
-  <si>
-    <t>US - Android Applikation Einsätze auf der Karte anzeigen (DB Zugriff mit WebService)</t>
-  </si>
-  <si>
-    <t>US - Android Appliaktion Stützpunkte auf Karte anzeigen (DB Zugriff mit WebService)</t>
-  </si>
-  <si>
     <t>US - Android Applikation Filteroptionen für Karte</t>
   </si>
   <si>
@@ -374,30 +362,6 @@
     <t>US - JavaFX Applikation Benutzer löschen</t>
   </si>
   <si>
-    <t>US - JavaFX Applikation Einsätze anzeigen (mit WebService)</t>
-  </si>
-  <si>
-    <t>US - JavaFX Applikation Einsätze verändern (mit WebService)</t>
-  </si>
-  <si>
-    <t>US - JavaFX Applikation Einsätze anlegen (mit WebService)</t>
-  </si>
-  <si>
-    <t>US - JavaFX Applikation Einsätze löschen (mit WebService)</t>
-  </si>
-  <si>
-    <t>US - JavaFX Applikation Stützpunkt anzeigen (mit WebService)</t>
-  </si>
-  <si>
-    <t>US - JavaFX Applikation Stützpunkt anlegen (mit WebService)</t>
-  </si>
-  <si>
-    <t>US - JavaFX Applikation Stützpunkt verändern (mit WebService)</t>
-  </si>
-  <si>
-    <t>US - JavaFX Applikation Stützpunkt löschen (mit WebService)</t>
-  </si>
-  <si>
     <t>US - Webservice Benutzer laden</t>
   </si>
   <si>
@@ -440,27 +404,9 @@
     <t>US - Tabellen mit Testdaten befüllen</t>
   </si>
   <si>
-    <t>US - JavaFX GUI Konzept anlegen</t>
-  </si>
-  <si>
     <t>US - Webservice Benutzer verändern</t>
   </si>
   <si>
-    <t>US - Android Applikation Einsätze als Testdaten anzeigen</t>
-  </si>
-  <si>
-    <t>US - Android Applikation Stützpunkte als Testdaten anzeigen</t>
-  </si>
-  <si>
-    <t>US - JavaFX Applikation Einsätze anzeigen</t>
-  </si>
-  <si>
-    <t>US - JavaFX Applikation Einsätze anlegen</t>
-  </si>
-  <si>
-    <t>US - JavaFX Applikation Einsätze verändern</t>
-  </si>
-  <si>
     <t xml:space="preserve">US - JavaFX Applikation Einsätze löschen </t>
   </si>
   <si>
@@ -468,13 +414,82 @@
   </si>
   <si>
     <t>US - Android GUI Konzept anlegen</t>
+  </si>
+  <si>
+    <t>JavaFX Applikation GUI Konzept Stützpunktverwaltung</t>
+  </si>
+  <si>
+    <t>JavaFX Applikation GUI Konzept Einsatzverwaltung</t>
+  </si>
+  <si>
+    <t>US - JavaFX GUI Konzept Stützpunktverwaltung</t>
+  </si>
+  <si>
+    <t>US - JavaFX GUI Konzept Einsatzverwaltung</t>
+  </si>
+  <si>
+    <t>US - Webservice Login</t>
+  </si>
+  <si>
+    <t>US - Webservice Register</t>
+  </si>
+  <si>
+    <t>US - Android Applikation Einsätze auf der Karte anzeigen</t>
+  </si>
+  <si>
+    <t>US - Android Appliaktion Stützpunkte auf Karte anzeigen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US - JavaFX Applikation Einsätze anzeigen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">US - JavaFX Applikation Einsätze anlegen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">US - JavaFX Applikation Einsätze verändern </t>
+  </si>
+  <si>
+    <t xml:space="preserve">US - JavaFX Applikation Stützpunkt anzeigen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">US - JavaFX Applikation Stützpunkt anlegen </t>
+  </si>
+  <si>
+    <t xml:space="preserve">US - JavaFX Applikation Stützpunkt verändern </t>
+  </si>
+  <si>
+    <t xml:space="preserve">US - JavaFX Applikation Stützpunkt löschen </t>
+  </si>
+  <si>
+    <t>Iteration</t>
+  </si>
+  <si>
+    <t>Legende</t>
+  </si>
+  <si>
+    <t>Wird in der Iteration 1  bearbeitet</t>
+  </si>
+  <si>
+    <t>Wird in der Iteration 2  bearbeitet</t>
+  </si>
+  <si>
+    <t>Wird in der Iteration 3  bearbeitet</t>
+  </si>
+  <si>
+    <t>Android Client US</t>
+  </si>
+  <si>
+    <t>JavaFX Client US</t>
+  </si>
+  <si>
+    <t>Webservice US</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -491,14 +506,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -506,7 +513,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -549,6 +556,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -571,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -582,16 +601,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1075,10 +1097,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2196546-D8CF-4C65-A015-BD5D70707281}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1270,97 +1292,107 @@
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>59</v>
+      <c r="A32" s="4" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>57</v>
+      <c r="A33" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>73</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>86</v>
       </c>
     </row>
@@ -1371,559 +1403,1031 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F10326-AF2F-4D5C-B1AD-D5133480706B}">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="100.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="82.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="82.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="60.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="52.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="55.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="60.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.5703125" customWidth="1"/>
+    <col min="9" max="9" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="11" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:13" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="9" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M1" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="B2" s="15">
+        <v>3</v>
+      </c>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="8" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K2" s="13"/>
+      <c r="M2" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="B3" s="15">
+        <v>3</v>
+      </c>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="8" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K3" s="13"/>
+      <c r="M3" s="17" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="B4" s="15">
+        <v>3</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="13"/>
+      <c r="K4" s="8" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="M4" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="16">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="8" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="M5" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="16">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="M6" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="16">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D7" s="13"/>
+      <c r="E7" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="M7" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B8" s="18">
+        <v>2</v>
+      </c>
+      <c r="C8" s="14"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="G8" s="13"/>
+      <c r="H8" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="I8" s="13"/>
+      <c r="J8" s="13"/>
+      <c r="K8" s="13"/>
+      <c r="M8" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="18">
+        <v>2</v>
+      </c>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="18">
+        <v>2</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="13"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" s="18">
+        <v>2</v>
+      </c>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="16">
+        <v>1</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="D12" s="13"/>
+      <c r="E12" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="B13" s="16">
+        <v>1</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E13" s="13"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="16">
+        <v>1</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" s="13"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+      <c r="K14" s="13"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" s="16">
+        <v>1</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D15" s="13"/>
+      <c r="E15" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B16" s="16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="13"/>
+      <c r="E16" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="B17" s="16">
+        <v>1</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="13"/>
+      <c r="E17" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="16">
+        <v>1</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="13"/>
+      <c r="E18" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19" s="18">
+        <v>2</v>
+      </c>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="B20" s="18">
+        <v>2</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B21" s="18">
+        <v>2</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G21" s="13"/>
+      <c r="H21" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B22" s="18">
+        <v>2</v>
+      </c>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="B10" s="17"/>
-      <c r="E10" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="E14" s="15"/>
-      <c r="G14" s="15"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F16" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
+      <c r="B23" s="16">
+        <v>1</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="E23" s="12"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+      <c r="K23" s="13"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B24" s="16">
+        <v>1</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="E24" s="12"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+      <c r="K24" s="13"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="B25" s="16">
+        <v>1</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="D25" s="13"/>
+      <c r="E25" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+      <c r="K25" s="13"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" s="16">
+        <v>1</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D26" s="13"/>
+      <c r="E26" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="B27" s="16">
+        <v>1</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="B28" s="18">
+        <v>2</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+      <c r="K28" s="13"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="E17" s="4" t="s">
+      <c r="B29" s="16">
+        <v>1</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="D29" s="11" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+      <c r="E29" s="13"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="13"/>
+      <c r="H29" s="13"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="13"/>
+      <c r="K29" s="13"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="B30" s="16">
+        <v>1</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="G18" s="4" t="s">
+      <c r="D30" s="11" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+      <c r="E30" s="13"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="13"/>
+      <c r="H30" s="13"/>
+      <c r="I30" s="13"/>
+      <c r="J30" s="13"/>
+      <c r="K30" s="13"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="B31" s="16">
+        <v>1</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="G19" s="4" t="s">
+      <c r="D31" s="12"/>
+      <c r="E31" s="11" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="F31" s="12"/>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B32" s="16">
+        <v>1</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="D32" s="12"/>
+      <c r="E32" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="F32" s="12"/>
+      <c r="G32" s="13"/>
+      <c r="H32" s="13"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="13"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="E20" s="4" t="s">
+      <c r="B33" s="16">
+        <v>1</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="D33" s="13"/>
+      <c r="E33" s="11" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="F33" s="12"/>
+      <c r="G33" s="13"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="13"/>
+      <c r="K33" s="13"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B34" s="16">
+        <v>1</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="D34" s="13"/>
+      <c r="E34" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" s="12"/>
+      <c r="G34" s="13"/>
+      <c r="H34" s="13"/>
+      <c r="I34" s="13"/>
+      <c r="J34" s="13"/>
+      <c r="K34" s="13"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B35" s="16">
+        <v>1</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" s="13"/>
+      <c r="E35" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="F35" s="12"/>
+      <c r="G35" s="13"/>
+      <c r="H35" s="13"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="13"/>
+      <c r="K35" s="13"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B36" s="16">
+        <v>1</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="B23" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="D36" s="13"/>
+      <c r="E36" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F36" s="12"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="13"/>
+      <c r="K36" s="13"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B37" s="18">
+        <v>2</v>
+      </c>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="G37" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="H37" s="12"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13"/>
+      <c r="K37" s="13"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B38" s="18">
+        <v>2</v>
+      </c>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+      <c r="E38" s="12"/>
+      <c r="F38" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="G38" s="11" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="10" t="s">
+      <c r="H38" s="12"/>
+      <c r="I38" s="13"/>
+      <c r="J38" s="13"/>
+      <c r="K38" s="13"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B39" s="18">
+        <v>2</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="G39" s="11" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
+      <c r="H39" s="12"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="B27" s="12" t="s">
+      <c r="B40" s="18">
+        <v>2</v>
+      </c>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
+      <c r="F40" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="G40" s="11" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="10" t="s">
+      <c r="H40" s="12"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="13"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B41" s="18">
+        <v>2</v>
+      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="G41" s="12"/>
+      <c r="H41" s="11" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="B29" s="12" t="s">
-        <v>135</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
+      <c r="I41" s="13"/>
+      <c r="J41" s="13"/>
+      <c r="K41" s="13"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B42" s="16">
+        <v>1</v>
+      </c>
+      <c r="C42" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="D42" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E42" s="13"/>
+      <c r="F42" s="12"/>
+      <c r="G42" s="12"/>
+      <c r="H42" s="12"/>
+      <c r="I42" s="13"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="13"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="B43" s="16">
+        <v>1</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="E43" s="13"/>
+      <c r="F43" s="12"/>
+      <c r="G43" s="12"/>
+      <c r="H43" s="12"/>
+      <c r="I43" s="13"/>
+      <c r="J43" s="13"/>
+      <c r="K43" s="13"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="E30" s="16" t="s">
+      <c r="B44" s="16">
+        <v>1</v>
+      </c>
+      <c r="C44" s="20" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+      <c r="D44" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+      <c r="G44" s="13"/>
+      <c r="H44" s="13"/>
+      <c r="I44" s="13"/>
+      <c r="J44" s="13"/>
+      <c r="K44" s="13"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="E31" s="16" t="s">
+      <c r="B45" s="16">
+        <v>1</v>
+      </c>
+      <c r="C45" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="20" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="E32" s="16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
-        <v>136</v>
-      </c>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="E33" s="16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="E34" s="15"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+      <c r="G45" s="13"/>
+      <c r="H45" s="13"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13"/>
+      <c r="K45" s="13"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B46" s="16">
+        <v>1</v>
+      </c>
+      <c r="C46" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D46" s="20" t="s">
         <v>125</v>
       </c>
-      <c r="E35" s="15"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="E36" s="15"/>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
-      <c r="G37" s="15"/>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="15"/>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>129</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="15"/>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>130</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
-      <c r="G40" s="15"/>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
-      <c r="G41" s="15"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
-      <c r="G42" s="15"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="B43" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="C43" s="6" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="B44" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="B45" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="C45" s="6" t="s">
-        <v>143</v>
-      </c>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+      <c r="G46" s="13"/>
+      <c r="H46" s="13"/>
+      <c r="I46" s="13"/>
+      <c r="J46" s="13"/>
+      <c r="K46" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>